<commit_message>
Fixed bug to return date from cell if date was calculated via function: eg: =today()
</commit_message>
<xml_diff>
--- a/test-data/data-loader/input/invoices.xlsx
+++ b/test-data/data-loader/input/invoices.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="14" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="8" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -384,15 +384,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>125640</xdr:rowOff>
+      <xdr:rowOff>116640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1078920</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19440</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>260640</xdr:rowOff>
+      <xdr:rowOff>251280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -407,8 +407,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="125640"/>
-          <a:ext cx="2989440" cy="296640"/>
+          <a:off x="135000" y="116640"/>
+          <a:ext cx="2999160" cy="296280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -429,18 +429,18 @@
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="false" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="topLeft" topLeftCell="A1" xSplit="0" ySplit="-1"/>
-      <selection activeCell="E5" activeCellId="0" pane="topLeft" sqref="E5"/>
+      <selection activeCell="E6" activeCellId="0" pane="topLeft" sqref="E6"/>
       <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.956862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9019607843137"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4549019607843"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5372549019608"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6705882352941"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.1450980392157"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0196078431373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5294117647059"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.7333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.2196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.8666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="34.4" outlineLevel="0" r="2">
@@ -469,8 +469,11 @@
       <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="5" t="n">
-        <v>41187</v>
+      <c r="E5" s="5" t="inlineStr">
+        <f aca="true">TODAY()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="F5" s="5"/>
     </row>

</xml_diff>

<commit_message>
Started code to support parents of landmarks that are empty
</commit_message>
<xml_diff>
--- a/test-data/data-loader/input/invoices.xlsx
+++ b/test-data/data-loader/input/invoices.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="173"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>INVOICE</t>
   </si>
@@ -104,6 +104,21 @@
   </si>
   <si>
     <t>My second product</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>#4 Some place</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>Some city</t>
+  </si>
+  <si>
+    <t>Some country</t>
   </si>
 </sst>
 </file>
@@ -194,46 +209,6 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -274,11 +249,51 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,10 +703,10 @@
     <sheetView showZeros="0" tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" activePane="bottomLeft"/>
       <selection activeCell="E43" sqref="E43"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="12"/>
     <col min="2" max="2" width="17"/>
@@ -703,385 +718,401 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="35.25">
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="13.7" customHeight="1">
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="1:6" ht="12.75">
-      <c r="A4" s="13" t="s">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" ht="12.75">
-      <c r="A5" s="13" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="16" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="17">
         <f ca="1">TODAY()</f>
-        <v>41192</v>
-      </c>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" ht="12.75">
-      <c r="A6" s="11" t="s">
+        <v>41194</v>
+      </c>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="16" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="19">
         <v>2</v>
       </c>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:6" ht="12.75">
-      <c r="A7" s="11" t="s">
+      <c r="F6" s="19"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
     </row>
     <row r="9" spans="1:6" ht="7.5" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="11" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="16" t="s">
+      <c r="B11" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="E11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="E12" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="B13" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="E13" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="16" spans="1:6" ht="12.75">
-      <c r="A16" s="17" t="s">
+      <c r="B14" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="E14" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="17" t="s">
+      <c r="E16" s="23"/>
+      <c r="F16" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="12.75">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="18"/>
-    </row>
-    <row r="19" spans="1:6" ht="12.75">
-      <c r="A19" s="17" t="s">
+    <row r="17" spans="1:6">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="17" t="s">
+      <c r="C19" s="23"/>
+      <c r="D19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A20" s="20">
+      <c r="A20" s="6">
         <v>1</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="21">
+      <c r="C20" s="25"/>
+      <c r="D20" s="7">
         <v>10</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="7">
         <v>1</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="7">
         <f t="shared" ref="F20:F31" si="0">IF(E20*D20=0,"",E20*D20)</f>
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A21" s="22">
+      <c r="A21" s="8">
         <v>2</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="23">
+      <c r="C21" s="26"/>
+      <c r="D21" s="9">
         <v>100</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="9">
         <v>0.5</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="9">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A22" s="20"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21" t="str">
+      <c r="A22" s="6"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A23" s="22"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23" t="str">
+      <c r="A23" s="8"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A24" s="20"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21" t="str">
+      <c r="A24" s="6"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A25" s="22"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23" t="str">
+      <c r="A25" s="8"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A26" s="20"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21" t="str">
+      <c r="A26" s="6"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A27" s="22"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23" t="str">
+      <c r="A27" s="8"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A28" s="20"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21" t="str">
+      <c r="A28" s="6"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A29" s="22"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23" t="str">
+      <c r="A29" s="8"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21" t="str">
+      <c r="A30" s="6"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A31" s="22"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23" t="str">
+      <c r="A31" s="8"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="12.75">
-      <c r="D32" s="2" t="s">
+    <row r="32" spans="1:6">
+      <c r="D32" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="21">
+      <c r="E32" s="27"/>
+      <c r="F32" s="7">
         <f>SUM(F20:F31)</f>
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="12.75">
-      <c r="A33" s="24" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="25">
+      <c r="E33" s="27"/>
+      <c r="F33" s="11">
         <v>0.05</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="12.75">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:6">
+      <c r="A34" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="2" t="s">
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="21">
+      <c r="E34" s="27"/>
+      <c r="F34" s="7">
         <f>IF(F32*F33=0,"0.00",F32*F33)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="12.75">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="29" t="s">
+    <row r="35" spans="1:6">
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="26">
+      <c r="E35" s="30"/>
+      <c r="F35" s="12">
         <f>IF(F32-F34=0,"0.00",F32-F34)</f>
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="12.75">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="29" t="s">
+    <row r="36" spans="1:6">
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="27">
+      <c r="E36" s="30"/>
+      <c r="F36" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="12.75">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="29" t="s">
+    <row r="37" spans="1:6">
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="28">
+      <c r="E37" s="30"/>
+      <c r="F37" s="14">
         <f>IF(F35-F36=0,"0.00",F35-F36)</f>
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="12.75">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="40" spans="1:6" ht="12.75">
-      <c r="A40" s="30" t="s">
+    <row r="38" spans="1:6">
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-    </row>
-    <row r="41" spans="1:6" ht="12.75">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="28"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="39">

</xml_diff>